<commit_message>
bugfixes, split villain deck schemes
Schemes fixed:
infinity gauntlet
fragmented realities
five families
breach parallel dimensions

extend promptdiscard to work on zones
extend playvillains for other decks and capture the deck running out
fix shard cloning
</commit_message>
<xml_diff>
--- a/data/villains.xlsx
+++ b/data/villains.xlsx
@@ -2639,10 +2639,10 @@
   <dimension ref="A1:AA446"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C413" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C250" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AA445" sqref="AA445"/>
+      <selection pane="bottomRight" activeCell="F268" sqref="F268"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11310,7 +11310,7 @@
         <v>4</v>
       </c>
       <c r="F266">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M266">
         <v>1</v>
@@ -11345,7 +11345,7 @@
         <v>5</v>
       </c>
       <c r="F267">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L267">
         <v>1</v>
@@ -11406,7 +11406,7 @@
         <v>3</v>
       </c>
       <c r="F269">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R269">
         <v>1</v>

</xml_diff>